<commit_message>
EPBDS-11727 Vertical conditions are matched instead of horizontal condition with the field of input object
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9226_SmartRulesMatching.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9226_SmartRulesMatching.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\BadLookup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B18913-EA51-4797-8040-2ED982CCA159}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E167FDE-E0C0-4A67-8FB8-97460623A161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30120" yWindow="6900" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7840" yWindow="2160" windowWidth="28800" windowHeight="15560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="24">
   <si>
     <t>My Value</t>
   </si>
@@ -49,12 +49,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t>Min</t>
-  </si>
-  <si>
-    <t>Max</t>
   </si>
   <si>
     <t>Marital Status</t>
@@ -516,7 +510,7 @@
   <dimension ref="B6:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,7 +520,7 @@
   <sheetData>
     <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -540,9 +534,7 @@
       <c r="C7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>6</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="1">
         <v>100</v>
       </c>
@@ -554,12 +546,8 @@
       <c r="B8" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
       <c r="E8" t="s">
         <v>1</v>
       </c>
@@ -637,7 +625,7 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B18" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -757,7 +745,7 @@
         <v>0</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D30" s="3">
         <v>100</v>
@@ -866,41 +854,41 @@
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
         <v>14</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>16</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>18</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
         <v>20</v>
-      </c>
-      <c r="F38" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
         <v>15</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>17</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>19</v>
       </c>
-      <c r="E39" t="s">
+      <c r="F39" t="s">
         <v>21</v>
-      </c>
-      <c r="F39" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.35">
@@ -916,41 +904,41 @@
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C45" t="s">
         <v>14</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>16</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>18</v>
       </c>
-      <c r="E45" t="s">
+      <c r="F45" t="s">
         <v>20</v>
-      </c>
-      <c r="F45" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
+        <v>13</v>
+      </c>
+      <c r="C46" t="s">
         <v>15</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>17</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>19</v>
       </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
         <v>21</v>
-      </c>
-      <c r="F46" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
@@ -980,17 +968,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C7:D8"/>
     <mergeCell ref="B29:G29"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="C30:C31"/>
     <mergeCell ref="D30:E30"/>
     <mergeCell ref="F30:G30"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="C19:D19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>